<commit_message>
slider de bateria adicionado
</commit_message>
<xml_diff>
--- a/novo_concatenado.xlsx
+++ b/novo_concatenado.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilherme.costa\Desktop\Thiago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7441DAE-E70D-40E0-B53C-B5708E603D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F526A39F-0C80-4DBD-BDD2-D2E9F2F949B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$1156</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -3931,7 +3934,7 @@
   <dimension ref="A1:C1156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15935,6 +15938,9 @@
       <c r="A1091" t="s">
         <v>48</v>
       </c>
+      <c r="C1091">
+        <v>0</v>
+      </c>
     </row>
     <row r="1092" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1092" t="s">
@@ -16652,6 +16658,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C1156" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>